<commit_message>
Update routines, builds, and documentation
</commit_message>
<xml_diff>
--- a/Documentation/DDCS Interfaces.xlsx
+++ b/Documentation/DDCS Interfaces.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileSharing readOnlyRecommended="1" userName="Theodore F. Fontana" algorithmName="SHA-512" hashValue="PeLuiZvChDFbeJ2O7EM8YanWy3CZMxAb5BfxIgLiOfeV4botsgnBXdQ631uERT2y0CCnrY8CWYzhofWnKXn3hw==" saltValue="jV0azMUps51V/fHaCjDXnw==" spinCount="100000"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfontana\Desktop\DSIO Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\imagetest\Product Versions\Maternity Tracker\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2040" windowHeight="7260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2040" windowHeight="7260"/>
   </bookViews>
   <sheets>
     <sheet name="Forms" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
   <si>
     <t>Display Name</t>
   </si>
@@ -81,11 +82,6 @@
     <t>Delivery Observatioins (Complete)</t>
   </si>
   <si>
-    <t>1. Generate Note isn't.
-2. Preview is bypassing validation on higher pages?
-3. Launch message for all oCNTs to state the pregnancy that will be used.</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -360,10 +356,6 @@
   </si>
   <si>
     <t>TdlgWheezing</t>
-  </si>
-  <si>
-    <t>1. The two items in red are part of pregnancy history but used to be their own dialogs that would leverage the M code which is no longer needed.
-2. Version 2 updates to 508 and is in a DEV complete state unless there is IHE work to be done which is M work so those items are not yet complete. Only these items that are DEV complete can be made QA complete.</t>
   </si>
   <si>
     <t>Vitals</t>
@@ -381,9 +373,6 @@
     <t>Breast Milk
 Bottle
 Formula</t>
-  </si>
-  <si>
-    <t>DSIO DDCS OBSERVATION CONFIG</t>
   </si>
   <si>
     <t>y</t>
@@ -442,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,8 +456,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -537,12 +532,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF666666"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF666666"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF666666"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -614,21 +624,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -641,12 +642,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -929,9 +970,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -970,17 +1011,17 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="H1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
       <c r="Q1" s="17" t="s">
         <v>3</v>
       </c>
@@ -1002,8 +1043,8 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>114</v>
+      <c r="G2" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="H2" s="9">
         <v>1</v>
@@ -1063,17 +1104,17 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>117</v>
+        <v>113</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
@@ -1104,17 +1145,17 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>117</v>
+        <v>113</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1153,17 +1194,17 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>117</v>
+        <v>113</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="H6" s="9">
         <v>1</v>
@@ -1195,34 +1236,10 @@
       <c r="Q6" s="20"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>115</v>
-      </c>
+      <c r="A8" s="13"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1">
@@ -1235,9 +1252,8 @@
     <filterColumn colId="13" showButton="0"/>
     <filterColumn colId="14" showButton="0"/>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="H1:P1"/>
-    <mergeCell ref="A9:P9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="DDCSForms\NursePostpartumMaternal.png"/>
@@ -1260,11 +1276,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,23 +1289,23 @@
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="12" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="12" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="36.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>1</v>
@@ -1307,59 +1323,61 @@
         <v>5</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+        <v>18</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="42"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="4" t="s">
+      <c r="D2" s="35">
+        <v>2</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="36"/>
+      <c r="I2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="37">
+        <v>1</v>
+      </c>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="42"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="9">
-        <v>1</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="26"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>26</v>
       </c>
       <c r="D3" s="6">
         <v>2</v>
@@ -1373,7 +1391,7 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="10">
         <v>1</v>
@@ -1381,181 +1399,187 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="28"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="N3" s="26"/>
+      <c r="O3" s="42"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="35">
+        <v>2</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="37">
+        <v>1</v>
+      </c>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="42"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="10">
-        <v>1</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="28"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="D5" s="29">
+        <v>2</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="28">
+        <v>1</v>
+      </c>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="42"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="26"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="C6" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="D6" s="35">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="37">
+        <v>1</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="42"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="29">
+        <v>2</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="28">
+        <v>1</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="42"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="28"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="9">
-        <v>1</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="D8" s="35">
+        <v>1</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="29" t="s">
+      <c r="I8" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="37">
+        <v>1</v>
+      </c>
+      <c r="K8" s="37">
+        <v>2</v>
+      </c>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="42"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="9">
-        <v>1</v>
-      </c>
-      <c r="K8" s="9">
-        <v>2</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
@@ -1569,7 +1593,7 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="10">
         <v>1</v>
@@ -1577,49 +1601,51 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="28"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="26"/>
+      <c r="O9" s="42"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="C10" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="D10" s="35">
+        <v>1</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="36"/>
+      <c r="I10" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="37">
+        <v>1</v>
+      </c>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="42"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="9">
-        <v>1</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>52</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
@@ -1631,11 +1657,11 @@
       <c r="G11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>53</v>
+      <c r="H11" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="10">
         <v>1</v>
@@ -1643,49 +1669,51 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="28"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="26"/>
+      <c r="O11" s="42"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="C12" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="D12" s="35">
+        <v>2</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="37">
+        <v>1</v>
+      </c>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="42"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="9">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="26"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -1697,63 +1725,65 @@
       <c r="G13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="28">
+        <v>1</v>
+      </c>
+      <c r="K13" s="28">
+        <v>2</v>
+      </c>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="42"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="31">
-        <v>1</v>
-      </c>
-      <c r="K13" s="31">
-        <v>2</v>
-      </c>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="28"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="C14" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="D14" s="35">
+        <v>2</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="36"/>
+      <c r="I14" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="37">
+        <v>1</v>
+      </c>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="42"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="9">
-        <v>1</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="26"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="25" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>66</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -1765,60 +1795,63 @@
       <c r="G15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>67</v>
+      <c r="H15" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="10">
         <v>1</v>
       </c>
+      <c r="K15" s="46"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="28"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="26"/>
+      <c r="O15" s="42"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="C16" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="D16" s="35">
+        <v>2</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="37">
+        <v>1</v>
+      </c>
+      <c r="K16" s="45"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="42"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="9">
-        <v>1</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="26"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>73</v>
       </c>
       <c r="D17" s="6">
         <v>2</v>
@@ -1832,7 +1865,7 @@
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="10">
         <v>1</v>
@@ -1840,51 +1873,53 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="28"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="26"/>
+      <c r="O17" s="42"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="C18" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="D18" s="35">
+        <v>1</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="37">
+        <v>1</v>
+      </c>
+      <c r="K18" s="37">
+        <v>2</v>
+      </c>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="42"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="9">
-        <v>1</v>
-      </c>
-      <c r="K18" s="9">
-        <v>2</v>
-      </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="26"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="C19" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>79</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -1897,10 +1932,10 @@
         <v>4</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="10">
         <v>1</v>
@@ -1910,49 +1945,51 @@
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="28"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="N19" s="26"/>
+      <c r="O19" s="42"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="C20" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="6">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="10">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="28"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="35">
+        <v>2</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="37">
+        <v>1</v>
+      </c>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="42"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="C21" s="25" t="s">
         <v>88</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>89</v>
       </c>
       <c r="D21" s="6">
         <v>2</v>
@@ -1966,7 +2003,7 @@
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" s="10">
         <v>1</v>
@@ -1974,260 +2011,268 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="28"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="26"/>
+      <c r="O21" s="42"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="C22" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="4">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="9">
-        <v>1</v>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="26"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="D22" s="35">
+        <v>2</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="37">
+        <v>1</v>
+      </c>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="42"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="D23" s="29">
+        <v>1</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="29" t="s">
+      <c r="I23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="28">
+        <v>1</v>
+      </c>
+      <c r="K23" s="28">
+        <v>2</v>
+      </c>
+      <c r="L23" s="28">
+        <v>3</v>
+      </c>
+      <c r="M23" s="28">
+        <v>4</v>
+      </c>
+      <c r="N23" s="33"/>
+      <c r="O23" s="42"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="9">
-        <v>2</v>
-      </c>
-      <c r="L23" s="9">
-        <v>3</v>
-      </c>
-      <c r="M23" s="9">
-        <v>4</v>
-      </c>
-      <c r="N23" s="26"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="C24" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="D24" s="35">
+        <v>1</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="37">
+        <v>1</v>
+      </c>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="42"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="10">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="28"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="D25" s="29">
+        <v>2</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="28">
+        <v>1</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="42"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="4">
-        <v>2</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="9">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="26"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="C26" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="D26" s="35">
+        <v>2</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="36"/>
+      <c r="I26" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="37">
+        <v>1</v>
+      </c>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="42"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="6">
-        <v>2</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="10">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="28"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="C27" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="D27" s="29">
+        <v>2</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="28">
+        <v>1</v>
+      </c>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="42"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="4">
-        <v>2</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="9">
-        <v>1</v>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="26"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="C28" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="6">
-        <v>2</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="10">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="28"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
+      <c r="D28" s="35">
+        <v>2</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="36"/>
+      <c r="I28" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="37">
+        <v>1</v>
+      </c>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="42"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="42"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="O30" s="42"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N28">
@@ -2238,9 +2283,8 @@
       <sortCondition ref="B1:B28"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="J1:M1"/>
-    <mergeCell ref="A31:N31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
@@ -2295,7 +2339,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2386,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="6">
         <v>2</v>
@@ -2363,7 +2407,7 @@
     </row>
     <row r="3" spans="1:9" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -2377,7 +2421,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H3" s="9">
         <v>2</v>
@@ -2386,7 +2430,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -2401,8 +2445,8 @@
       <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>113</v>
+      <c r="G4" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="H4" s="10">
         <v>3</v>
@@ -2410,25 +2454,20 @@
       <c r="I4" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I4"/>
-  <mergeCells count="1">
-    <mergeCell ref="A7:H7"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="DDCSVitals\V1.png"/>
     <hyperlink ref="H3" r:id="rId2" display="DDCSVitals\V2.png"/>

</xml_diff>